<commit_message>
feat(agent-improvements): Update template and filling for agent and ocd reports
</commit_message>
<xml_diff>
--- a/assets/pod_report_template.xlsx
+++ b/assets/pod_report_template.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Work/Sunrise Frequency Reporting/Sunrise-Frequency-Reporting/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsoldin/Documents/Work/Sunrise/Sunrise-Frequency-Reporting/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5038B9-2493-9344-A284-3F17E4E43867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBB31E-BDB3-A04E-A4B6-50C782AD9486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="760" windowWidth="27640" windowHeight="18880" xr2:uid="{61660ABD-414E-DC4A-816F-BEBC35F6E77A}"/>
+    <workbookView xWindow="10460" yWindow="3860" windowWidth="31200" windowHeight="20820" xr2:uid="{61660ABD-414E-DC4A-816F-BEBC35F6E77A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Physical" sheetId="2" r:id="rId1"/>
+    <sheet name="Verbal" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>date_time</t>
-  </si>
-  <si>
-    <t>MISSING POD REPORT</t>
   </si>
   <si>
     <t>num_missing</t>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>agent_name</t>
+  </si>
+  <si>
+    <t>MISSING PHYSICAL POD REPORT</t>
+  </si>
+  <si>
+    <t>MISSING VERBAL POD REPORT</t>
   </si>
 </sst>
 </file>
@@ -136,11 +139,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -164,15 +167,64 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D0E3B12-D29C-594A-B3DF-C3EAC6CA0913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177800" y="177800"/>
+          <a:ext cx="4533900" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -195,7 +247,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="165100" y="139700"/>
+          <a:off x="177800" y="177800"/>
           <a:ext cx="4533900" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -524,94 +576,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B98DE08-80F5-F344-A985-032ED542FD35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C785AC-0FA4-7E4E-8E86-5D4990053698}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="52.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
-        <v>3</v>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="5"/>
       <c r="O7" s="3"/>
@@ -619,12 +672,12 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -636,4 +689,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B98DE08-80F5-F344-A985-032ED542FD35}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed data extraction, template and pod/acd reports
</commit_message>
<xml_diff>
--- a/assets/pod_report_template.xlsx
+++ b/assets/pod_report_template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsoldin/Documents/Work/Sunrise/Sunrise-Frequency-Reporting/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Work/Sunrise Frequency Reporting/Sunrise-Frequency-Reporting/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBB31E-BDB3-A04E-A4B6-50C782AD9486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA67FE54-43F5-D047-9CFC-DBF04D0BD2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="3860" windowWidth="31200" windowHeight="20820" xr2:uid="{61660ABD-414E-DC4A-816F-BEBC35F6E77A}"/>
+    <workbookView xWindow="30460" yWindow="3380" windowWidth="31200" windowHeight="20820" activeTab="2" xr2:uid="{61660ABD-414E-DC4A-816F-BEBC35F6E77A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Physical" sheetId="2" r:id="rId1"/>
-    <sheet name="Verbal" sheetId="1" r:id="rId2"/>
+    <sheet name="Verbal Missing" sheetId="2" r:id="rId1"/>
+    <sheet name="Image Missing" sheetId="1" r:id="rId2"/>
+    <sheet name="Verbal Not Captured" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>date_time</t>
   </si>
@@ -50,10 +51,13 @@
     <t>agent_name</t>
   </si>
   <si>
-    <t>MISSING PHYSICAL POD REPORT</t>
+    <t>MISSING VERBAL POD REPORT</t>
   </si>
   <si>
-    <t>MISSING VERBAL POD REPORT</t>
+    <t>MISSING IMAGE POD REPORT</t>
+  </si>
+  <si>
+    <t>VERBAL NOT CAPTURED POD REPORT</t>
   </si>
 </sst>
 </file>
@@ -232,6 +236,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF6FA14-0920-9E44-9DE3-B81512EA47CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177800" y="177800"/>
+          <a:ext cx="4533900" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE1FAABF-A837-E643-86FB-92107343EA4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -579,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C785AC-0FA4-7E4E-8E86-5D4990053698}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +749,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,4 +858,120 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4ED79EB-E775-AA4A-AC1C-482E32F8D02D}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>